<commit_message>
Update dict for metrics
</commit_message>
<xml_diff>
--- a/Config/todo.xlsx
+++ b/Config/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SmileFactory\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4DD9CFF-18A7-4A8D-9B07-3D5213118314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B935CD-400B-4F55-9224-6926DD1F7A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{258C9B79-B8B1-4B8F-A161-CB4A531C84BE}"/>
   </bookViews>
@@ -593,10 +593,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -975,16 +975,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B47C9DC-005E-4351-A8FC-B988ACE426BA}">
   <dimension ref="A1:D324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N264" sqref="N264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3881,6 +3881,140 @@
     </row>
   </sheetData>
   <mergeCells count="150">
+    <mergeCell ref="A163:A216"/>
+    <mergeCell ref="A217:A270"/>
+    <mergeCell ref="A271:A324"/>
+    <mergeCell ref="B1:B9"/>
+    <mergeCell ref="B10:B18"/>
+    <mergeCell ref="B19:B27"/>
+    <mergeCell ref="B28:B36"/>
+    <mergeCell ref="B37:B45"/>
+    <mergeCell ref="B46:B54"/>
+    <mergeCell ref="A1:A54"/>
+    <mergeCell ref="A55:A108"/>
+    <mergeCell ref="A109:A162"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B55:B63"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="B64:B72"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="B91:B99"/>
+    <mergeCell ref="C91:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="B100:B108"/>
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="C106:C108"/>
+    <mergeCell ref="B73:B81"/>
+    <mergeCell ref="C73:C75"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="B82:B90"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="C85:C87"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="B127:B135"/>
+    <mergeCell ref="C127:C129"/>
+    <mergeCell ref="C130:C132"/>
+    <mergeCell ref="C133:C135"/>
+    <mergeCell ref="B136:B144"/>
+    <mergeCell ref="C136:C138"/>
+    <mergeCell ref="C139:C141"/>
+    <mergeCell ref="C142:C144"/>
+    <mergeCell ref="B109:B117"/>
+    <mergeCell ref="C109:C111"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="B118:B126"/>
+    <mergeCell ref="C118:C120"/>
+    <mergeCell ref="C121:C123"/>
+    <mergeCell ref="C124:C126"/>
+    <mergeCell ref="B163:B171"/>
+    <mergeCell ref="C163:C165"/>
+    <mergeCell ref="C166:C168"/>
+    <mergeCell ref="C169:C171"/>
+    <mergeCell ref="B172:B180"/>
+    <mergeCell ref="C172:C174"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="C178:C180"/>
+    <mergeCell ref="B145:B153"/>
+    <mergeCell ref="C145:C147"/>
+    <mergeCell ref="C148:C150"/>
+    <mergeCell ref="C151:C153"/>
+    <mergeCell ref="B154:B162"/>
+    <mergeCell ref="C154:C156"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="C160:C162"/>
+    <mergeCell ref="B199:B207"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="C202:C204"/>
+    <mergeCell ref="C205:C207"/>
+    <mergeCell ref="B208:B216"/>
+    <mergeCell ref="C208:C210"/>
+    <mergeCell ref="C211:C213"/>
+    <mergeCell ref="C214:C216"/>
+    <mergeCell ref="B181:B189"/>
+    <mergeCell ref="C181:C183"/>
+    <mergeCell ref="C184:C186"/>
+    <mergeCell ref="C187:C189"/>
+    <mergeCell ref="B190:B198"/>
+    <mergeCell ref="C190:C192"/>
+    <mergeCell ref="C193:C195"/>
+    <mergeCell ref="C196:C198"/>
+    <mergeCell ref="B235:B243"/>
+    <mergeCell ref="C235:C237"/>
+    <mergeCell ref="C238:C240"/>
+    <mergeCell ref="C241:C243"/>
+    <mergeCell ref="B244:B252"/>
+    <mergeCell ref="C244:C246"/>
+    <mergeCell ref="C247:C249"/>
+    <mergeCell ref="C250:C252"/>
+    <mergeCell ref="B217:B225"/>
+    <mergeCell ref="C217:C219"/>
+    <mergeCell ref="C220:C222"/>
+    <mergeCell ref="C223:C225"/>
+    <mergeCell ref="B226:B234"/>
+    <mergeCell ref="C226:C228"/>
+    <mergeCell ref="C229:C231"/>
+    <mergeCell ref="C232:C234"/>
+    <mergeCell ref="B271:B279"/>
+    <mergeCell ref="C271:C273"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="C277:C279"/>
+    <mergeCell ref="B280:B288"/>
+    <mergeCell ref="C280:C282"/>
+    <mergeCell ref="C283:C285"/>
+    <mergeCell ref="C286:C288"/>
+    <mergeCell ref="B253:B261"/>
+    <mergeCell ref="C253:C255"/>
+    <mergeCell ref="C256:C258"/>
+    <mergeCell ref="C259:C261"/>
+    <mergeCell ref="B262:B270"/>
+    <mergeCell ref="C262:C264"/>
+    <mergeCell ref="C265:C267"/>
+    <mergeCell ref="C268:C270"/>
     <mergeCell ref="B307:B315"/>
     <mergeCell ref="C307:C309"/>
     <mergeCell ref="C310:C312"/>
@@ -3897,140 +4031,6 @@
     <mergeCell ref="C298:C300"/>
     <mergeCell ref="C301:C303"/>
     <mergeCell ref="C304:C306"/>
-    <mergeCell ref="B271:B279"/>
-    <mergeCell ref="C271:C273"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="C277:C279"/>
-    <mergeCell ref="B280:B288"/>
-    <mergeCell ref="C280:C282"/>
-    <mergeCell ref="C283:C285"/>
-    <mergeCell ref="C286:C288"/>
-    <mergeCell ref="B253:B261"/>
-    <mergeCell ref="C253:C255"/>
-    <mergeCell ref="C256:C258"/>
-    <mergeCell ref="C259:C261"/>
-    <mergeCell ref="B262:B270"/>
-    <mergeCell ref="C262:C264"/>
-    <mergeCell ref="C265:C267"/>
-    <mergeCell ref="C268:C270"/>
-    <mergeCell ref="B235:B243"/>
-    <mergeCell ref="C235:C237"/>
-    <mergeCell ref="C238:C240"/>
-    <mergeCell ref="C241:C243"/>
-    <mergeCell ref="B244:B252"/>
-    <mergeCell ref="C244:C246"/>
-    <mergeCell ref="C247:C249"/>
-    <mergeCell ref="C250:C252"/>
-    <mergeCell ref="B217:B225"/>
-    <mergeCell ref="C217:C219"/>
-    <mergeCell ref="C220:C222"/>
-    <mergeCell ref="C223:C225"/>
-    <mergeCell ref="B226:B234"/>
-    <mergeCell ref="C226:C228"/>
-    <mergeCell ref="C229:C231"/>
-    <mergeCell ref="C232:C234"/>
-    <mergeCell ref="B199:B207"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="C202:C204"/>
-    <mergeCell ref="C205:C207"/>
-    <mergeCell ref="B208:B216"/>
-    <mergeCell ref="C208:C210"/>
-    <mergeCell ref="C211:C213"/>
-    <mergeCell ref="C214:C216"/>
-    <mergeCell ref="B181:B189"/>
-    <mergeCell ref="C181:C183"/>
-    <mergeCell ref="C184:C186"/>
-    <mergeCell ref="C187:C189"/>
-    <mergeCell ref="B190:B198"/>
-    <mergeCell ref="C190:C192"/>
-    <mergeCell ref="C193:C195"/>
-    <mergeCell ref="C196:C198"/>
-    <mergeCell ref="B163:B171"/>
-    <mergeCell ref="C163:C165"/>
-    <mergeCell ref="C166:C168"/>
-    <mergeCell ref="C169:C171"/>
-    <mergeCell ref="B172:B180"/>
-    <mergeCell ref="C172:C174"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="C178:C180"/>
-    <mergeCell ref="B145:B153"/>
-    <mergeCell ref="C145:C147"/>
-    <mergeCell ref="C148:C150"/>
-    <mergeCell ref="C151:C153"/>
-    <mergeCell ref="B154:B162"/>
-    <mergeCell ref="C154:C156"/>
-    <mergeCell ref="C157:C159"/>
-    <mergeCell ref="C160:C162"/>
-    <mergeCell ref="B127:B135"/>
-    <mergeCell ref="C127:C129"/>
-    <mergeCell ref="C130:C132"/>
-    <mergeCell ref="C133:C135"/>
-    <mergeCell ref="B136:B144"/>
-    <mergeCell ref="C136:C138"/>
-    <mergeCell ref="C139:C141"/>
-    <mergeCell ref="C142:C144"/>
-    <mergeCell ref="B109:B117"/>
-    <mergeCell ref="C109:C111"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="B118:B126"/>
-    <mergeCell ref="C118:C120"/>
-    <mergeCell ref="C121:C123"/>
-    <mergeCell ref="C124:C126"/>
-    <mergeCell ref="B91:B99"/>
-    <mergeCell ref="C91:C93"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="B100:B108"/>
-    <mergeCell ref="C100:C102"/>
-    <mergeCell ref="C103:C105"/>
-    <mergeCell ref="C106:C108"/>
-    <mergeCell ref="B73:B81"/>
-    <mergeCell ref="C73:C75"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="C79:C81"/>
-    <mergeCell ref="B82:B90"/>
-    <mergeCell ref="C82:C84"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="B55:B63"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="B64:B72"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="C70:C72"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B1:B9"/>
-    <mergeCell ref="B10:B18"/>
-    <mergeCell ref="B19:B27"/>
-    <mergeCell ref="B28:B36"/>
-    <mergeCell ref="B37:B45"/>
-    <mergeCell ref="B46:B54"/>
-    <mergeCell ref="A1:A54"/>
-    <mergeCell ref="A55:A108"/>
-    <mergeCell ref="A109:A162"/>
-    <mergeCell ref="A163:A216"/>
-    <mergeCell ref="A217:A270"/>
-    <mergeCell ref="A271:A324"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>